<commit_message>
Report bug fix 2
</commit_message>
<xml_diff>
--- a/rating_list.xlsx
+++ b/rating_list.xlsx
@@ -516,11 +516,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Окунева Анна Александровна </t>
+          <t>Сагацкая Варвара Николаевна</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
@@ -529,11 +529,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Васильев Андрей Витальевич</t>
+          <t>Галкина Елизавета Денисовна</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9">
@@ -542,11 +542,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Сагацкая Варвара Николаевна</t>
+          <t>Шепелева Ева Владимирована</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
@@ -555,11 +555,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Алексеев Александр Сергеевич </t>
+          <t xml:space="preserve">Окунева Анна Александровна </t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
@@ -568,11 +568,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Михайлова Милана Сергеевна </t>
+          <t>Васильев Андрей Витальевич</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -581,11 +581,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Егоров Матвей Александрович </t>
+          <t>Яковлев Александр Иванович</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13">
@@ -594,11 +594,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Тимофеев Александр Владимирович </t>
+          <t>Носов Ростислав Дмитриевич</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14">
@@ -607,11 +607,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Смирова Наталья Алексеевна</t>
+          <t>Баков Геннадий Владимирович</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15">
@@ -620,11 +620,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Галкина Елизавета Денисовна</t>
+          <t xml:space="preserve">Алексеев Александр Сергеевич </t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
@@ -633,11 +633,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Шепелева Ева Владимирована</t>
+          <t xml:space="preserve">Михайлова Милана Сергеевна </t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17">
@@ -646,11 +646,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Баков Геннадий Владимирович</t>
+          <t xml:space="preserve">Егоров Матвей Александрович </t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
@@ -659,11 +659,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Наумов Игорь Вячеславович</t>
+          <t xml:space="preserve">Тимофеев Александр Владимирович </t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
@@ -672,11 +672,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Яковлев Александр Иванович</t>
+          <t>Русанова Василиса Антоновна</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
@@ -685,11 +685,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Поляков Консантин Дмитриевич</t>
+          <t>Наумов Игорь Вячеславович</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
@@ -698,11 +698,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Носов Ростислав Дмитриевич</t>
+          <t>Смирова Наталья Алексеевна</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
@@ -711,11 +711,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Саладайкин Лев Николаевич</t>
+          <t>Поляков Консантин Дмитриевич</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
@@ -724,11 +724,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Русанова Василиса Антоновна</t>
+          <t>Саладайкин Лев Николаевич</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">

</xml_diff>